<commit_message>
created matrix at the bottom
</commit_message>
<xml_diff>
--- a/(11-17-18) calculated vectors from test.xlsx
+++ b/(11-17-18) calculated vectors from test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{0741BED3-7AC7-41D0-8AF0-BD98E51FCD4B}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{373568AE-BB34-4FA4-B935-1F355B055844}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>h1</t>
   </si>
@@ -89,6 +89,12 @@
   <si>
     <t>Level 1</t>
   </si>
+  <si>
+    <t xml:space="preserve">Matrix </t>
+  </si>
+  <si>
+    <t>Matrix Transpose</t>
+  </si>
 </sst>
 </file>
 
@@ -103,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:I9" si="0">2 * B2</f>
+        <f t="shared" ref="B9:H9" si="0">2 * B2</f>
         <v>4</v>
       </c>
       <c r="C9">
@@ -635,7 +648,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ref="A10:I10" si="1">2 * A3</f>
+        <f t="shared" ref="A10:H10" si="1">2 * A3</f>
         <v>4</v>
       </c>
       <c r="B10">
@@ -673,7 +686,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:I11" si="2">2 * A4</f>
+        <f t="shared" ref="A11:H11" si="2">2 * A4</f>
         <v>6</v>
       </c>
       <c r="B11">
@@ -711,7 +724,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" ref="A12:I12" si="3">2 * A5</f>
+        <f t="shared" ref="A12:H12" si="3">2 * A5</f>
         <v>8</v>
       </c>
       <c r="B12">
@@ -749,7 +762,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" ref="A13:I13" si="4">2 * A6</f>
+        <f t="shared" ref="A13:H13" si="4">2 * A6</f>
         <v>10</v>
       </c>
       <c r="B13">
@@ -1086,7 +1099,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ref="A27:G28" si="12">A20 * 2</f>
+        <f t="shared" ref="A27:G27" si="12">A20 * 2</f>
         <v>272</v>
       </c>
       <c r="B27">
@@ -1229,7 +1242,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ref="A34:F35" si="17">$I27</f>
+        <f t="shared" ref="A34:F34" si="17">$I27</f>
         <v>1904</v>
       </c>
       <c r="B34">
@@ -1440,7 +1453,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" ref="A45:E50" si="25">$H38</f>
+        <f t="shared" ref="A45:E48" si="25">$H38</f>
         <v>14784</v>
       </c>
       <c r="B45">
@@ -1582,7 +1595,7 @@
         <v>29568</v>
       </c>
       <c r="G52">
-        <f t="shared" ref="G52:G56" si="28">SUM(A52:E52)</f>
+        <f t="shared" ref="G52:G53" si="28">SUM(A52:E52)</f>
         <v>147840</v>
       </c>
     </row>
@@ -1773,7 +1786,7 @@
         <v>241920</v>
       </c>
       <c r="B65">
-        <f t="shared" ref="B65:E65" si="34">2 * B58</f>
+        <f t="shared" ref="B65:D65" si="34">2 * B58</f>
         <v>241920</v>
       </c>
       <c r="C65">
@@ -1791,7 +1804,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" ref="A66:E66" si="35">2 * A59</f>
+        <f t="shared" ref="A66:D66" si="35">2 * A59</f>
         <v>295680</v>
       </c>
       <c r="B66">
@@ -1813,7 +1826,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" ref="A67:E67" si="37">2 * A60</f>
+        <f t="shared" ref="A67:D67" si="37">2 * A60</f>
         <v>349440</v>
       </c>
       <c r="B67">
@@ -1835,7 +1848,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" ref="A68:E68" si="38">2 * A61</f>
+        <f t="shared" ref="A68:D68" si="38">2 * A61</f>
         <v>403200</v>
       </c>
       <c r="B68">
@@ -1857,7 +1870,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" ref="A69:E69" si="39">2 * A62</f>
+        <f t="shared" ref="A69:D69" si="39">2 * A62</f>
         <v>456960</v>
       </c>
       <c r="B69">
@@ -1898,7 +1911,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" ref="A73:C77" si="41">$F66</f>
+        <f t="shared" ref="A73:C76" si="41">$F66</f>
         <v>1182720</v>
       </c>
       <c r="B73">
@@ -1966,7 +1979,7 @@
         <v>1935360</v>
       </c>
       <c r="B79">
-        <f t="shared" ref="B79:D79" si="42">2 * B72</f>
+        <f t="shared" ref="B79:C79" si="42">2 * B72</f>
         <v>1935360</v>
       </c>
       <c r="C79">
@@ -1980,7 +1993,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" ref="A80:D80" si="43">2 * A73</f>
+        <f t="shared" ref="A80:C80" si="43">2 * A73</f>
         <v>2365440</v>
       </c>
       <c r="B80">
@@ -1996,9 +2009,9 @@
         <v>7096320</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" ref="A81:D81" si="44">2 * A74</f>
+        <f t="shared" ref="A81:C81" si="44">2 * A74</f>
         <v>2795520</v>
       </c>
       <c r="B81">
@@ -2014,9 +2027,9 @@
         <v>8386560</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" ref="A82:D82" si="45">2 * A75</f>
+        <f t="shared" ref="A82:C82" si="45">2 * A75</f>
         <v>3225600</v>
       </c>
       <c r="B82">
@@ -2032,9 +2045,9 @@
         <v>9676800</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" ref="A83:D83" si="46">2 * A76</f>
+        <f t="shared" ref="A83:C83" si="46">2 * A76</f>
         <v>3655680</v>
       </c>
       <c r="B83">
@@ -2050,62 +2063,178 @@
         <v>10967040</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="E85" t="s">
+        <v>22</v>
+      </c>
+      <c r="K85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <f>$E79</f>
         <v>5806080</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <f>$E79</f>
         <v>5806080</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <f>A86</f>
+        <v>5806080</v>
+      </c>
+      <c r="M86">
+        <f>B86</f>
+        <v>5806080</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <f t="shared" ref="A87:B87" si="47">$E80</f>
         <v>7096320</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <f t="shared" si="47"/>
         <v>7096320</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="E87">
+        <f>$L$86</f>
+        <v>5806080</v>
+      </c>
+      <c r="F87">
+        <f>$L$87</f>
+        <v>7096320</v>
+      </c>
+      <c r="G87">
+        <f>$L$88</f>
+        <v>8386560</v>
+      </c>
+      <c r="H87">
+        <f>$L$89</f>
+        <v>9676800</v>
+      </c>
+      <c r="I87">
+        <f>$L$90</f>
+        <v>10967040</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <f>A87</f>
+        <v>7096320</v>
+      </c>
+      <c r="M87">
+        <f>B87</f>
+        <v>7096320</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <f t="shared" ref="A88:B88" si="48">$E81</f>
         <v>8386560</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <f t="shared" si="48"/>
         <v>8386560</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="E88">
+        <f>$L$86</f>
+        <v>5806080</v>
+      </c>
+      <c r="F88">
+        <f>$L$87</f>
+        <v>7096320</v>
+      </c>
+      <c r="G88">
+        <f>$L$88</f>
+        <v>8386560</v>
+      </c>
+      <c r="H88">
+        <f>$L$89</f>
+        <v>9676800</v>
+      </c>
+      <c r="I88">
+        <f>$L$90</f>
+        <v>10967040</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <f>A88</f>
+        <v>8386560</v>
+      </c>
+      <c r="M88">
+        <f>B88</f>
+        <v>8386560</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <f t="shared" ref="A89:B89" si="49">$E82</f>
         <v>9676800</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <f t="shared" si="49"/>
         <v>9676800</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <f>A89</f>
+        <v>9676800</v>
+      </c>
+      <c r="M89">
+        <f>B89</f>
+        <v>9676800</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <f t="shared" ref="A90:B90" si="50">$E83</f>
         <v>10967040</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <f t="shared" si="50"/>
         <v>10967040</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <f>A90</f>
+        <v>10967040</v>
+      </c>
+      <c r="M90">
+        <f>B90</f>
+        <v>10967040</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2113,13 +2242,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>2 * A86</f>
         <v>11612160</v>
       </c>
       <c r="B93">
-        <f t="shared" ref="B93:D93" si="51">2 * B86</f>
+        <f t="shared" ref="B93" si="51">2 * B86</f>
         <v>11612160</v>
       </c>
       <c r="D93">
@@ -2127,9 +2256,9 @@
         <v>23224320</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" ref="A94:D94" si="52">2 * A87</f>
+        <f t="shared" ref="A94:B94" si="52">2 * A87</f>
         <v>14192640</v>
       </c>
       <c r="B94">
@@ -2141,9 +2270,9 @@
         <v>28385280</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" ref="A95:D95" si="54">2 * A88</f>
+        <f t="shared" ref="A95:B95" si="54">2 * A88</f>
         <v>16773120</v>
       </c>
       <c r="B95">
@@ -2155,9 +2284,9 @@
         <v>33546240</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" ref="A96:D96" si="55">2 * A89</f>
+        <f t="shared" ref="A96:B96" si="55">2 * A89</f>
         <v>19353600</v>
       </c>
       <c r="B96">
@@ -2171,7 +2300,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" ref="A97:D97" si="56">2 * A90</f>
+        <f t="shared" ref="A97:B97" si="56">2 * A90</f>
         <v>21934080</v>
       </c>
       <c r="B97">
@@ -2196,7 +2325,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" ref="A101:A105" si="57">D94</f>
+        <f t="shared" ref="A101:A104" si="57">D94</f>
         <v>28385280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created matrix and put it in row-echelon form. I did not solve it yet
</commit_message>
<xml_diff>
--- a/(11-17-18) calculated vectors from test.xlsx
+++ b/(11-17-18) calculated vectors from test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{373568AE-BB34-4FA4-B935-1F355B055844}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{4EF3BB8F-2A37-440D-BBAD-5E441A877A9D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>h1</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Matrix Transpose</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Matrix </t>
+  </si>
+  <si>
+    <t>Tranpose * B</t>
   </si>
 </sst>
 </file>
@@ -418,13 +427,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="Q98" sqref="Q98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2009,7 +2022,7 @@
         <v>7096320</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" ref="A81:C81" si="44">2 * A74</f>
         <v>2795520</v>
@@ -2027,7 +2040,7 @@
         <v>8386560</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" ref="A82:C82" si="45">2 * A75</f>
         <v>3225600</v>
@@ -2045,7 +2058,7 @@
         <v>9676800</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" ref="A83:C83" si="46">2 * A76</f>
         <v>3655680</v>
@@ -2063,7 +2076,7 @@
         <v>10967040</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2073,8 +2086,14 @@
       <c r="K85" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O85" t="s">
+        <v>23</v>
+      </c>
+      <c r="S85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f>$E79</f>
         <v>5806080</v>
@@ -2102,21 +2121,35 @@
         <v>1</v>
       </c>
       <c r="L86">
-        <f>A86</f>
+        <f t="shared" ref="L86:M90" si="47">A86</f>
         <v>5806080</v>
       </c>
       <c r="M86">
-        <f>B86</f>
+        <f t="shared" si="47"/>
         <v>5806080</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O86">
+        <v>5</v>
+      </c>
+      <c r="P86">
+        <f>SUM(L86:L90)</f>
+        <v>41932800</v>
+      </c>
+      <c r="Q86">
+        <f>SUM(M86:M90)</f>
+        <v>41932800</v>
+      </c>
+      <c r="S86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" ref="A87:B87" si="47">$E80</f>
+        <f t="shared" ref="A87:B87" si="48">$E80</f>
         <v>7096320</v>
       </c>
       <c r="B87" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>7096320</v>
       </c>
       <c r="E87">
@@ -2143,21 +2176,36 @@
         <v>1</v>
       </c>
       <c r="L87">
-        <f>A87</f>
+        <f t="shared" si="47"/>
         <v>7096320</v>
       </c>
       <c r="M87">
-        <f>B87</f>
+        <f t="shared" si="47"/>
         <v>7096320</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O87">
+        <f>SUM(E87:I87)</f>
+        <v>41932800</v>
+      </c>
+      <c r="P87">
+        <f>($E$87*$L$86)+($F$87*$L$87)+($G$87*$L$88)+($H$87*$L$89)+($I$87*$L$89)</f>
+        <v>354169022054400</v>
+      </c>
+      <c r="Q87">
+        <f>($E$87*$L$86)+($F$87*$L$87)+($G$87*$L$88)+($H$87*$L$89)+($I$87*$L$89)</f>
+        <v>354169022054400</v>
+      </c>
+      <c r="S87">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" ref="A88:B88" si="48">$E81</f>
+        <f t="shared" ref="A88:B88" si="49">$E81</f>
         <v>8386560</v>
       </c>
       <c r="B88" s="1">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>8386560</v>
       </c>
       <c r="E88">
@@ -2184,57 +2232,78 @@
         <v>1</v>
       </c>
       <c r="L88">
-        <f>A88</f>
+        <f t="shared" si="47"/>
         <v>8386560</v>
       </c>
       <c r="M88">
-        <f>B88</f>
+        <f t="shared" si="47"/>
         <v>8386560</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O88">
+        <f>SUM(E88:I88)</f>
+        <v>41932800</v>
+      </c>
+      <c r="P88">
+        <f>($E$87*$L$86)+($F$87*$L$87)+($G$87*$L$88)+($H$87*$L$89)+($I$87*$L$89)</f>
+        <v>354169022054400</v>
+      </c>
+      <c r="Q88">
+        <f>($E$87*$L$86)+($F$87*$L$87)+($G$87*$L$88)+($H$87*$L$89)+($I$87*$L$89)</f>
+        <v>354169022054400</v>
+      </c>
+      <c r="S88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" ref="A89:B89" si="49">$E82</f>
+        <f t="shared" ref="A89:B89" si="50">$E82</f>
         <v>9676800</v>
       </c>
       <c r="B89" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>9676800</v>
       </c>
       <c r="K89">
         <v>1</v>
       </c>
       <c r="L89">
-        <f>A89</f>
+        <f t="shared" si="47"/>
         <v>9676800</v>
       </c>
       <c r="M89">
-        <f>B89</f>
+        <f t="shared" si="47"/>
         <v>9676800</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S89">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" ref="A90:B90" si="50">$E83</f>
+        <f t="shared" ref="A90:B90" si="51">$E83</f>
         <v>10967040</v>
       </c>
       <c r="B90" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>10967040</v>
       </c>
       <c r="K90">
         <v>1</v>
       </c>
       <c r="L90">
-        <f>A90</f>
+        <f t="shared" si="47"/>
         <v>10967040</v>
       </c>
       <c r="M90">
-        <f>B90</f>
+        <f t="shared" si="47"/>
         <v>10967040</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S90">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2242,13 +2311,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>2 * A86</f>
         <v>11612160</v>
       </c>
       <c r="B93">
-        <f t="shared" ref="B93" si="51">2 * B86</f>
+        <f t="shared" ref="B93" si="52">2 * B86</f>
         <v>11612160</v>
       </c>
       <c r="D93">
@@ -2256,94 +2325,187 @@
         <v>23224320</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" ref="A94:B94" si="52">2 * A87</f>
+        <f t="shared" ref="A94:B94" si="53">2 * A87</f>
         <v>14192640</v>
       </c>
       <c r="B94">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>14192640</v>
       </c>
       <c r="D94">
-        <f t="shared" ref="D94:D97" si="53">SUM(A94:C94)</f>
+        <f t="shared" ref="D94:D97" si="54">SUM(A94:C94)</f>
         <v>28385280</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>22</v>
+      </c>
+      <c r="M94" t="s">
+        <v>24</v>
+      </c>
+      <c r="O94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" ref="A95:B95" si="54">2 * A88</f>
+        <f t="shared" ref="A95:B95" si="55">2 * A88</f>
         <v>16773120</v>
       </c>
       <c r="B95">
+        <f t="shared" si="55"/>
+        <v>16773120</v>
+      </c>
+      <c r="D95">
         <f t="shared" si="54"/>
-        <v>16773120</v>
-      </c>
-      <c r="D95">
-        <f t="shared" si="53"/>
         <v>33546240</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <v>9</v>
+      </c>
+      <c r="O95">
+        <f>SUM(M95:M99)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" ref="A96:B96" si="55">2 * A89</f>
+        <f t="shared" ref="A96:B96" si="56">2 * A89</f>
         <v>19353600</v>
       </c>
       <c r="B96">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>19353600</v>
       </c>
       <c r="D96">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>38707200</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <f>$L$86</f>
+        <v>5806080</v>
+      </c>
+      <c r="H96">
+        <f>$L$87</f>
+        <v>7096320</v>
+      </c>
+      <c r="I96">
+        <f>$L$88</f>
+        <v>8386560</v>
+      </c>
+      <c r="J96">
+        <f>$L$89</f>
+        <v>9676800</v>
+      </c>
+      <c r="K96">
+        <f>$L$90</f>
+        <v>10967040</v>
+      </c>
+      <c r="M96">
+        <v>10</v>
+      </c>
+      <c r="O96">
+        <f xml:space="preserve"> ($G$96 * $M$95) + ($H$96 * $M$96) + ($I$96 *$M$97) + ($J$96 * $M$98) + ($K$96 *$M$99)</f>
+        <v>474163200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" ref="A97:B97" si="56">2 * A90</f>
+        <f t="shared" ref="A97:B97" si="57">2 * A90</f>
         <v>21934080</v>
       </c>
       <c r="B97">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>21934080</v>
       </c>
       <c r="D97">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>43868160</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <f>$L$86</f>
+        <v>5806080</v>
+      </c>
+      <c r="H97">
+        <f>$L$87</f>
+        <v>7096320</v>
+      </c>
+      <c r="I97">
+        <f>$L$88</f>
+        <v>8386560</v>
+      </c>
+      <c r="J97">
+        <f>$L$89</f>
+        <v>9676800</v>
+      </c>
+      <c r="K97">
+        <f>$L$90</f>
+        <v>10967040</v>
+      </c>
+      <c r="M97">
+        <v>11</v>
+      </c>
+      <c r="O97">
+        <f xml:space="preserve"> ($G$96 * $M$95) + ($H$96 * $M$96) + ($I$96 *$M$97) + ($J$96 * $M$98) + ($K$96 *$M$99)</f>
+        <v>474163200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M98">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>D93</f>
         <v>23224320</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" ref="A101:A104" si="57">D94</f>
+        <f t="shared" ref="A101:A104" si="58">D94</f>
         <v>28385280</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>33546240</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>38707200</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>43868160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the neuro network is able to determine the weight for the lowest level. Now a method need to be made to determine the rest of the weights for the neuro network.
</commit_message>
<xml_diff>
--- a/(11-17-18) calculated vectors from test.xlsx
+++ b/(11-17-18) calculated vectors from test.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="173" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{4EF3BB8F-2A37-440D-BBAD-5E441A877A9D}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="11_F25DC773A252ABEACE02EC10639D4E6C5ADE589F" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{B3FE7364-3C1B-4D7A-8E03-8264A26D8019}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>h1</t>
   </si>
@@ -103,6 +103,33 @@
   </si>
   <si>
     <t>Tranpose * B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Matrix </t>
+  </si>
+  <si>
+    <t>Mult and Sub 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The original values of test </t>
+  </si>
+  <si>
+    <t>Mult and Sub 2</t>
+  </si>
+  <si>
+    <t>Mult 1 and Sub 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divide by 1 </t>
+  </si>
+  <si>
+    <t>Mult and Sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset </t>
+  </si>
+  <si>
+    <t>Reset</t>
   </si>
 </sst>
 </file>
@@ -118,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +155,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,9 +183,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,19 +479,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S104"/>
+  <dimension ref="A1:T126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="Q98" sqref="Q98"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +528,16 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -496,8 +565,14 @@
       <c r="I2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -525,8 +600,14 @@
       <c r="I3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -554,8 +635,14 @@
       <c r="I4">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -583,8 +670,14 @@
       <c r="I5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -612,8 +705,22 @@
       <c r="I6">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -621,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>2 * A2</f>
         <v>2</v>
@@ -659,7 +766,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ref="A10:H10" si="1">2 * A3</f>
         <v>4</v>
@@ -697,7 +804,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:H11" si="2">2 * A4</f>
         <v>6</v>
@@ -735,7 +842,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ref="A12:H12" si="3">2 * A5</f>
         <v>8</v>
@@ -773,7 +880,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ref="A13:H13" si="4">2 * A6</f>
         <v>10</v>
@@ -811,12 +918,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <f xml:space="preserve"> $J9</f>
         <v>72</v>
@@ -2425,7 +2532,7 @@
         <v>474163200</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" ref="A97:B97" si="57">2 * A90</f>
         <v>21934080</v>
@@ -2466,12 +2573,12 @@
         <v>474163200</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M98">
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -2479,37 +2586,623 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>D93</f>
         <v>23224320</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" ref="A101:A104" si="58">D94</f>
         <v>28385280</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="58"/>
         <v>33546240</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="58"/>
         <v>38707200</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>26</v>
+      </c>
+      <c r="I103" t="s">
+        <v>27</v>
+      </c>
+      <c r="N103" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="58"/>
         <v>43868160</v>
       </c>
+      <c r="D104">
+        <v>5</v>
+      </c>
+      <c r="E104">
+        <v>-1362736721171.96</v>
+      </c>
+      <c r="F104">
+        <v>-1312514297178.8401</v>
+      </c>
+      <c r="G104">
+        <v>108</v>
+      </c>
+      <c r="I104">
+        <f xml:space="preserve"> $D$105 /$D$104 * D104</f>
+        <v>-1362736721171.96</v>
+      </c>
+      <c r="J104">
+        <f t="shared" ref="J104:L104" si="59" xml:space="preserve"> $D$105 /$D$104 * E104</f>
+        <v>3.7141027424610081E+23</v>
+      </c>
+      <c r="K104">
+        <f xml:space="preserve"> $D$105 /$D$104 * F104</f>
+        <v>3.5772228596576242E+23</v>
+      </c>
+      <c r="L104">
+        <f xml:space="preserve"> $D$105 /$D$104 * G104</f>
+        <v>-29435113177314.336</v>
+      </c>
+      <c r="N104">
+        <f xml:space="preserve"> ($I$106 / $I$104) * I104</f>
+        <v>-1312514297178.8401</v>
+      </c>
+      <c r="O104">
+        <f t="shared" ref="O104:Q104" si="60" xml:space="preserve"> ($I$106 / $I$104) * J104</f>
+        <v>3.5772228596576235E+23</v>
+      </c>
+      <c r="P104">
+        <f t="shared" si="60"/>
+        <v>3.445387560597729E+23</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="60"/>
+        <v>-28350308819062.945</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>-1362736721171.96</v>
+      </c>
+      <c r="E105" s="5">
+        <v>6.9522734812106004E+24</v>
+      </c>
+      <c r="F105" s="5">
+        <v>6.4305349444302398E+24</v>
+      </c>
+      <c r="G105">
+        <v>-29983205004856.398</v>
+      </c>
+      <c r="I105">
+        <f>D105 - I104</f>
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <f>E105 - J104</f>
+        <v>6.5808632069644992E+24</v>
+      </c>
+      <c r="K105">
+        <f t="shared" ref="J105:L105" si="61">F105 - K104</f>
+        <v>6.0728126584644777E+24</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="61"/>
+        <v>-548091827542.0625</v>
+      </c>
+      <c r="N105">
+        <f xml:space="preserve"> I105</f>
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <f t="shared" ref="O105:Q105" si="62" xml:space="preserve"> J105</f>
+        <v>6.5808632069644992E+24</v>
+      </c>
+      <c r="P105">
+        <f t="shared" si="62"/>
+        <v>6.0728126584644777E+24</v>
+      </c>
+      <c r="Q105">
+        <f t="shared" si="62"/>
+        <v>-548091827542.0625</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>-1312514297178.8401</v>
+      </c>
+      <c r="E106" s="5">
+        <v>6.4305349444302398E+24</v>
+      </c>
+      <c r="F106" s="5">
+        <v>5.9650776403376397E+24</v>
+      </c>
+      <c r="G106">
+        <v>-24185764424849.199</v>
+      </c>
+      <c r="I106">
+        <f xml:space="preserve"> D106</f>
+        <v>-1312514297178.8401</v>
+      </c>
+      <c r="J106">
+        <f t="shared" ref="J106:L106" si="63" xml:space="preserve"> E106</f>
+        <v>6.4305349444302398E+24</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="63"/>
+        <v>5.9650776403376397E+24</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="63"/>
+        <v>-24185764424849.199</v>
+      </c>
+      <c r="N106">
+        <f xml:space="preserve"> I106 - N104</f>
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <f t="shared" ref="O106:Q106" si="64" xml:space="preserve"> J106 - O104</f>
+        <v>6.0728126584644777E+24</v>
+      </c>
+      <c r="P106">
+        <f t="shared" si="64"/>
+        <v>5.6205388842778668E+24</v>
+      </c>
+      <c r="Q106">
+        <f t="shared" si="64"/>
+        <v>4164544394213.7461</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I108" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J108" s="7"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <f>N104</f>
+        <v>-1312514297178.8401</v>
+      </c>
+      <c r="J109">
+        <f t="shared" ref="J109:L110" si="65">O104</f>
+        <v>3.5772228596576235E+23</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="65"/>
+        <v>3.445387560597729E+23</v>
+      </c>
+      <c r="L109">
+        <f t="shared" si="65"/>
+        <v>-28350308819062.945</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <f xml:space="preserve"> ($O$106 / $O$105) * N105</f>
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <f t="shared" ref="J110:L110" si="66" xml:space="preserve"> ($O$106 / $O$105) * O105</f>
+        <v>6.0728126584644777E+24</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="66"/>
+        <v>5.6039842228869695E+24</v>
+      </c>
+      <c r="L110">
+        <f t="shared" si="66"/>
+        <v>-505778479755.64551</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <f xml:space="preserve"> N106 - I110</f>
+        <v>0</v>
+      </c>
+      <c r="J111">
+        <f t="shared" ref="J111:L111" si="67" xml:space="preserve"> O106 - J110</f>
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="67"/>
+        <v>1.6554661390897373E+22</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="67"/>
+        <v>4670322873969.3916</v>
+      </c>
+    </row>
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D113" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I113" t="s">
+        <v>32</v>
+      </c>
+      <c r="N113" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <f xml:space="preserve"> (1 / $I$109) * I109</f>
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <f xml:space="preserve"> (1 / $I$109) * J109</f>
+        <v>-272547344234.39194</v>
+      </c>
+      <c r="F114">
+        <f xml:space="preserve"> (1 / $I$109) * K109</f>
+        <v>-262502859435.76801</v>
+      </c>
+      <c r="G114">
+        <f xml:space="preserve"> (1 / $I$109) * L109</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="I114">
+        <f xml:space="preserve"> D114 - I115</f>
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <f t="shared" ref="J114:L114" si="68" xml:space="preserve"> E114 - J115</f>
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="68"/>
+        <v>-10996497725.365784</v>
+      </c>
+      <c r="L114">
+        <f t="shared" si="68"/>
+        <v>21.577300702461784</v>
+      </c>
+      <c r="N114">
+        <f>I114</f>
+        <v>1</v>
+      </c>
+      <c r="O114">
+        <f t="shared" ref="O114:Q114" si="69">J114</f>
+        <v>0</v>
+      </c>
+      <c r="P114">
+        <f t="shared" si="69"/>
+        <v>-10996497725.365784</v>
+      </c>
+      <c r="Q114">
+        <f t="shared" si="69"/>
+        <v>21.577300702461784</v>
+      </c>
+    </row>
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <f xml:space="preserve"> (1 / $J$110) * J110</f>
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <f xml:space="preserve"> (1 / $J$110) * K110</f>
+        <v>0.92279879819377597</v>
+      </c>
+      <c r="G115">
+        <f xml:space="preserve"> (1 / $J$110) * L110</f>
+        <v>-8.3285704368086431E-14</v>
+      </c>
+      <c r="I115">
+        <f xml:space="preserve"> $E$114 * D115</f>
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <f t="shared" ref="J115:L115" si="70" xml:space="preserve"> $E$114 * E115</f>
+        <v>-272547344234.39194</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="70"/>
+        <v>-251506361710.40222</v>
+      </c>
+      <c r="L115">
+        <f t="shared" si="70"/>
+        <v>2.2699297538212652E-2</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115">
+        <f>J115 / $J$115</f>
+        <v>1</v>
+      </c>
+      <c r="P115">
+        <f t="shared" ref="P115:Q115" si="71">K115 / $J$115</f>
+        <v>0.92279879819377597</v>
+      </c>
+      <c r="Q115">
+        <f t="shared" si="71"/>
+        <v>-8.3285704368086431E-14</v>
+      </c>
+    </row>
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f xml:space="preserve"> (1 / $K$111) * K111</f>
+        <v>1</v>
+      </c>
+      <c r="G116">
+        <f xml:space="preserve"> (1 / $K$111) * L111</f>
+        <v>2.8211527639806525E-10</v>
+      </c>
+      <c r="I116">
+        <f>D116</f>
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <f t="shared" ref="J116:L116" si="72">E116</f>
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="72"/>
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="72"/>
+        <v>2.8211527639806525E-10</v>
+      </c>
+      <c r="N116">
+        <f xml:space="preserve"> I116</f>
+        <v>0</v>
+      </c>
+      <c r="O116">
+        <f t="shared" ref="O116:Q116" si="73" xml:space="preserve"> J116</f>
+        <v>0</v>
+      </c>
+      <c r="P116">
+        <f t="shared" si="73"/>
+        <v>1</v>
+      </c>
+      <c r="Q116">
+        <f t="shared" si="73"/>
+        <v>2.8211527639806525E-10</v>
+      </c>
+    </row>
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I118" t="s">
+        <v>32</v>
+      </c>
+      <c r="N118" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <f xml:space="preserve"> N114 - I121</f>
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <f t="shared" ref="J119:L119" si="74" xml:space="preserve"> O114 - J121</f>
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="74"/>
+        <v>24.679580697664047</v>
+      </c>
+      <c r="N119">
+        <f>I119</f>
+        <v>1</v>
+      </c>
+      <c r="O119">
+        <f t="shared" ref="O119:Q119" si="75">J119</f>
+        <v>0</v>
+      </c>
+      <c r="P119">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="Q119">
+        <f t="shared" si="75"/>
+        <v>24.679580697664047</v>
+      </c>
+    </row>
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I120">
+        <f>D115</f>
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <f t="shared" ref="J120:L120" si="76">E115</f>
+        <v>1</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="76"/>
+        <v>0.92279879819377597</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="76"/>
+        <v>-8.3285704368086431E-14</v>
+      </c>
+      <c r="N120">
+        <f xml:space="preserve"> I120</f>
+        <v>0</v>
+      </c>
+      <c r="O120">
+        <f t="shared" ref="O120:Q120" si="77" xml:space="preserve"> J120</f>
+        <v>1</v>
+      </c>
+      <c r="P120">
+        <f t="shared" si="77"/>
+        <v>0.92279879819377597</v>
+      </c>
+      <c r="Q120">
+        <f t="shared" si="77"/>
+        <v>-8.3285704368086431E-14</v>
+      </c>
+    </row>
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I121">
+        <f xml:space="preserve"> $P$114 * N116</f>
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <f t="shared" ref="J121:L121" si="78" xml:space="preserve"> $P$114 * O116</f>
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <f xml:space="preserve"> $P$114 * P116</f>
+        <v>-10996497725.365784</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="78"/>
+        <v>-3.1022799952022639</v>
+      </c>
+      <c r="N121">
+        <f xml:space="preserve"> D116</f>
+        <v>0</v>
+      </c>
+      <c r="O121">
+        <f t="shared" ref="O121:Q121" si="79" xml:space="preserve"> E116</f>
+        <v>0</v>
+      </c>
+      <c r="P121">
+        <f t="shared" si="79"/>
+        <v>1</v>
+      </c>
+      <c r="Q121">
+        <f t="shared" si="79"/>
+        <v>2.8211527639806525E-10</v>
+      </c>
+    </row>
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I123" t="s">
+        <v>32</v>
+      </c>
+      <c r="N123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I124">
+        <f xml:space="preserve"> N119</f>
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <f t="shared" ref="J124:L124" si="80" xml:space="preserve"> O119</f>
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="80"/>
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="80"/>
+        <v>24.679580697664047</v>
+      </c>
+      <c r="N124">
+        <f xml:space="preserve"> I124</f>
+        <v>1</v>
+      </c>
+      <c r="O124">
+        <f t="shared" ref="O124:Q125" si="81" xml:space="preserve"> J124</f>
+        <v>0</v>
+      </c>
+      <c r="P124">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="Q124" s="8">
+        <f t="shared" si="81"/>
+        <v>24.679580697664047</v>
+      </c>
+    </row>
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I125">
+        <f xml:space="preserve"> N120 - I126</f>
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <f t="shared" ref="J125:L125" si="82" xml:space="preserve"> O120 - J126</f>
+        <v>1</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="82"/>
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="82"/>
+        <v>-2.6041892371660765E-10</v>
+      </c>
+      <c r="N125">
+        <f xml:space="preserve"> I125</f>
+        <v>0</v>
+      </c>
+      <c r="O125">
+        <f t="shared" si="81"/>
+        <v>1</v>
+      </c>
+      <c r="P125">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="Q125" s="8">
+        <f t="shared" si="81"/>
+        <v>-2.6041892371660765E-10</v>
+      </c>
+    </row>
+    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I126">
+        <f xml:space="preserve"> $P$120 * N121</f>
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <f t="shared" ref="J126:L126" si="83" xml:space="preserve"> $P$120 * O121</f>
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="83"/>
+        <v>0.92279879819377597</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="83"/>
+        <v>2.6033563801223956E-10</v>
+      </c>
+      <c r="N126">
+        <f xml:space="preserve"> D116</f>
+        <v>0</v>
+      </c>
+      <c r="O126">
+        <f t="shared" ref="O126:Q126" si="84" xml:space="preserve"> E116</f>
+        <v>0</v>
+      </c>
+      <c r="P126">
+        <f t="shared" si="84"/>
+        <v>1</v>
+      </c>
+      <c r="Q126" s="8">
+        <f t="shared" si="84"/>
+        <v>2.8211527639806525E-10</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K1:M3"/>
+    <mergeCell ref="I108:J108"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>